<commit_message>
Changed tok and chem
</commit_message>
<xml_diff>
--- a/Chemistry/draft/data/data.xlsx
+++ b/Chemistry/draft/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder2021\IAProjects\Chemistry\draft\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88B3C15-2424-46E9-B4D0-7665327E4799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE924DA-DD5A-4D57-85CF-2C1739A4C1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="484" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="13" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -367,7 +367,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,6 +382,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent 1 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -16550,15 +16553,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:M365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J187" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I215" sqref="I215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.75" customWidth="1"/>
     <col min="4" max="4" width="15.75" customWidth="1"/>
-    <col min="5" max="12" width="13.75" customWidth="1"/>
+    <col min="5" max="9" width="16.25" customWidth="1"/>
+    <col min="10" max="12" width="13.75" customWidth="1"/>
     <col min="15" max="15" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16584,26 +16588,26 @@
       </c>
     </row>
     <row r="6" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="26" t="s">
+      <c r="H6" s="22"/>
+      <c r="I6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="26" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="26"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
@@ -17599,26 +17603,26 @@
       </c>
     </row>
     <row r="49" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24" t="s">
+      <c r="D49" s="22"/>
+      <c r="E49" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26" t="s">
+      <c r="F49" s="24"/>
+      <c r="G49" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H49" s="23"/>
-      <c r="I49" s="26" t="s">
+      <c r="H49" s="22"/>
+      <c r="I49" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J49" s="23"/>
-      <c r="K49" s="26" t="s">
+      <c r="J49" s="22"/>
+      <c r="K49" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="L49" s="26"/>
+      <c r="L49" s="25"/>
     </row>
     <row r="50" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" s="7" t="s">
@@ -18884,26 +18888,26 @@
       </c>
     </row>
     <row r="90" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C90" s="22" t="s">
+      <c r="C90" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D90" s="23"/>
-      <c r="E90" s="24" t="s">
+      <c r="D90" s="22"/>
+      <c r="E90" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F90" s="25"/>
-      <c r="G90" s="26" t="s">
+      <c r="F90" s="24"/>
+      <c r="G90" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H90" s="23"/>
-      <c r="I90" s="26" t="s">
+      <c r="H90" s="22"/>
+      <c r="I90" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J90" s="23"/>
-      <c r="K90" s="26" t="s">
+      <c r="J90" s="22"/>
+      <c r="K90" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="L90" s="26"/>
+      <c r="L90" s="25"/>
     </row>
     <row r="91" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C91" s="8" t="s">
@@ -21379,12 +21383,23 @@
       <c r="G169" s="3"/>
       <c r="H169" s="2"/>
     </row>
-    <row r="217" spans="4:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D217" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="4:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F218" s="7"/>
+      <c r="G218" s="7"/>
+    </row>
+    <row r="219" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F219" s="29"/>
+      <c r="G219" s="29"/>
+      <c r="H219" s="29"/>
+      <c r="I219" s="29"/>
+      <c r="J219" s="7"/>
+    </row>
+    <row r="220" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D220" s="20"/>
       <c r="E220" s="8" t="s">
         <v>19</v>
@@ -21398,12 +21413,18 @@
       <c r="H220" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I220" s="8" t="s">
+      <c r="I220" s="27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="221" spans="4:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D221" s="21" t="s">
+      <c r="J220" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K220" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="221" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D221" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E221">
@@ -21418,27 +21439,20 @@
       <c r="H221">
         <v>-295.73</v>
       </c>
-      <c r="I221">
+      <c r="I221" s="26">
         <v>-296.98</v>
       </c>
-    </row>
-    <row r="222" spans="4:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D222" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E222">
+      <c r="J221">
         <f>AVERAGE(E221:I221)</f>
         <v>-292.012</v>
       </c>
-    </row>
-    <row r="223" spans="4:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D223" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E223">
+      <c r="K221">
         <f>0.5*(MAX(E221:I221)-MIN(E221:I221))</f>
         <v>21.695000000000022</v>
       </c>
+    </row>
+    <row r="224" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E224" s="7"/>
     </row>
     <row r="226" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D226" s="6" t="s">
@@ -22521,21 +22535,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="K90:L90"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>